<commit_message>
Got matlab to reproduce the same charts as excel
</commit_message>
<xml_diff>
--- a/Step4.xlsx
+++ b/Step4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F29BD282-4649-43EF-BA8B-7393A06A71CD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D37704A7-2177-4514-AD70-3C3545A29879}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12037,7 +12037,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C88710-04DD-4DFC-8CAA-CA590D2C39F5}">
-  <dimension ref="A1:F321"/>
+  <dimension ref="A1:F380"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -12078,7 +12078,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>3.1152647975077881E-3</v>
@@ -12098,7 +12098,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>6.2305295950155761E-3</v>
@@ -12118,7 +12118,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>9.3457943925233638E-3</v>
@@ -12138,7 +12138,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>1.2461059190031152E-2</v>
@@ -12158,7 +12158,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>1.5576323987538941E-2</v>
@@ -12178,7 +12178,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>1.8691588785046728E-2</v>
@@ -12198,7 +12198,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>2.1806853582554516E-2</v>
@@ -12218,7 +12218,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>2.4922118380062305E-2</v>
@@ -12238,7 +12238,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D10">
         <v>2.8037383177570093E-2</v>
@@ -12258,7 +12258,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>3.1152647975077882E-2</v>
@@ -12278,7 +12278,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="D12">
         <v>3.4267912772585667E-2</v>
@@ -12298,7 +12298,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="D13">
         <v>3.7383177570093455E-2</v>
@@ -12318,7 +12318,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>4.0498442367601244E-2</v>
@@ -12338,7 +12338,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D15">
         <v>4.3613707165109032E-2</v>
@@ -12358,7 +12358,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="D16">
         <v>4.6728971962616821E-2</v>
@@ -12378,7 +12378,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D17">
         <v>4.9844236760124609E-2</v>
@@ -12398,7 +12398,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C18">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D18">
         <v>5.2959501557632398E-2</v>
@@ -12418,7 +12418,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="D19">
         <v>5.6074766355140186E-2</v>
@@ -12438,7 +12438,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C20">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="D20">
         <v>5.9190031152647975E-2</v>
@@ -12458,7 +12458,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="D21">
         <v>6.2305295950155763E-2</v>
@@ -12478,7 +12478,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="D22">
         <v>6.5420560747663545E-2</v>
@@ -12498,7 +12498,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C23">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="D23">
         <v>6.8535825545171333E-2</v>
@@ -12518,7 +12518,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C24">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>7.1651090342679122E-2</v>
@@ -12538,7 +12538,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C25">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D25">
         <v>7.476635514018691E-2</v>
@@ -12558,7 +12558,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>7.7881619937694699E-2</v>
@@ -12578,7 +12578,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C27">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="D27">
         <v>8.0996884735202487E-2</v>
@@ -12598,7 +12598,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C28">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="D28">
         <v>8.4112149532710276E-2</v>
@@ -12618,7 +12618,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C29">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="D29">
         <v>8.7227414330218064E-2</v>
@@ -12638,7 +12638,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C30">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D30">
         <v>9.0342679127725853E-2</v>
@@ -12658,7 +12658,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C31">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D31">
         <v>9.3457943925233641E-2</v>
@@ -12678,7 +12678,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C32">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="D32">
         <v>9.657320872274143E-2</v>
@@ -12698,7 +12698,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C33">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D33">
         <v>9.9688473520249218E-2</v>
@@ -12718,7 +12718,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C34">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="D34">
         <v>0.10280373831775701</v>
@@ -12738,7 +12738,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C35">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D35">
         <v>0.1059190031152648</v>
@@ -12758,7 +12758,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C36">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="D36">
         <v>0.10903426791277258</v>
@@ -12778,7 +12778,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C37">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="D37">
         <v>0.11214953271028037</v>
@@ -12798,7 +12798,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C38">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="D38">
         <v>0.11526479750778816</v>
@@ -12818,7 +12818,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C39">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D39">
         <v>0.11838006230529595</v>
@@ -12838,7 +12838,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C40">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="D40">
         <v>0.12149532710280374</v>
@@ -12858,7 +12858,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C41">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="D41">
         <v>0.12461059190031153</v>
@@ -12878,7 +12878,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C42">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="D42">
         <v>0.1277258566978193</v>
@@ -12898,7 +12898,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C43">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="D43">
         <v>0.13084112149532709</v>
@@ -12918,7 +12918,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C44">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="D44">
         <v>0.13395638629283488</v>
@@ -12938,7 +12938,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C45">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="D45">
         <v>0.13707165109034267</v>
@@ -12958,7 +12958,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C46">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="D46">
         <v>0.14018691588785046</v>
@@ -12978,7 +12978,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C47">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="D47">
         <v>0.14330218068535824</v>
@@ -12998,7 +12998,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C48">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D48">
         <v>0.14641744548286603</v>
@@ -13018,7 +13018,7 @@
         <v>4.2484952420493594</v>
       </c>
       <c r="C49">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="D49">
         <v>0.14953271028037382</v>
@@ -13038,7 +13038,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C50">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="D50">
         <v>0.15264797507788161</v>
@@ -13058,7 +13058,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C51">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="D51">
         <v>0.1557632398753894</v>
@@ -13078,7 +13078,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C52">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="D52">
         <v>0.15887850467289719</v>
@@ -13098,7 +13098,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C53">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="D53">
         <v>0.16199376947040497</v>
@@ -13118,7 +13118,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C54">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="D54">
         <v>0.16510903426791276</v>
@@ -13138,7 +13138,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C55">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="D55">
         <v>0.16822429906542055</v>
@@ -13158,7 +13158,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C56">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="D56">
         <v>0.17133956386292834</v>
@@ -13178,7 +13178,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C57">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="D57">
         <v>0.17445482866043613</v>
@@ -13198,7 +13198,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C58">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="D58">
         <v>0.17757009345794392</v>
@@ -13218,7 +13218,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C59">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="D59">
         <v>0.18068535825545171</v>
@@ -13238,7 +13238,7 @@
         <v>4.2626798770413155</v>
       </c>
       <c r="C60">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="D60">
         <v>0.18380062305295949</v>
@@ -13258,7 +13258,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C61">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="D61">
         <v>0.18691588785046728</v>
@@ -13278,7 +13278,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C62">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="D62">
         <v>0.19003115264797507</v>
@@ -13298,7 +13298,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C63">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="D63">
         <v>0.19314641744548286</v>
@@ -13318,7 +13318,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C64">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="D64">
         <v>0.19626168224299065</v>
@@ -13338,7 +13338,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C65">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="D65">
         <v>0.19937694704049844</v>
@@ -13358,7 +13358,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C66">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="D66">
         <v>0.20249221183800623</v>
@@ -13378,7 +13378,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C67">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="D67">
         <v>0.20560747663551401</v>
@@ -13398,7 +13398,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C68">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="D68">
         <v>0.2087227414330218</v>
@@ -13418,7 +13418,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C69">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="D69">
         <v>0.21183800623052959</v>
@@ -13438,7 +13438,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C70">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="D70">
         <v>0.21495327102803738</v>
@@ -13458,7 +13458,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C71">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="D71">
         <v>0.21806853582554517</v>
@@ -13478,7 +13478,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C72">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="D72">
         <v>0.22118380062305296</v>
@@ -13498,7 +13498,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C73">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="D73">
         <v>0.22429906542056074</v>
@@ -13518,7 +13518,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C74">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="D74">
         <v>0.22741433021806853</v>
@@ -13538,7 +13538,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C75">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="D75">
         <v>0.23052959501557632</v>
@@ -13558,7 +13558,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C76">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="D76">
         <v>0.23364485981308411</v>
@@ -13578,7 +13578,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C77">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="D77">
         <v>0.2367601246105919</v>
@@ -13598,7 +13598,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C78">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="D78">
         <v>0.23987538940809969</v>
@@ -13618,7 +13618,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C79">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="D79">
         <v>0.24299065420560748</v>
@@ -13638,7 +13638,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C80">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="D80">
         <v>0.24610591900311526</v>
@@ -13658,7 +13658,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C81">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="D81">
         <v>0.24922118380062305</v>
@@ -13678,7 +13678,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C82">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="D82">
         <v>0.25233644859813081</v>
@@ -13698,7 +13698,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C83">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="D83">
         <v>0.2554517133956386</v>
@@ -13718,7 +13718,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C84">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="D84">
         <v>0.25856697819314639</v>
@@ -13738,7 +13738,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C85">
-        <v>84</v>
+        <v>143</v>
       </c>
       <c r="D85">
         <v>0.26168224299065418</v>
@@ -13758,7 +13758,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C86">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="D86">
         <v>0.26479750778816197</v>
@@ -13778,7 +13778,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C87">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="D87">
         <v>0.26791277258566976</v>
@@ -13798,7 +13798,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C88">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="D88">
         <v>0.27102803738317754</v>
@@ -13818,7 +13818,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C89">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="D89">
         <v>0.27414330218068533</v>
@@ -13838,7 +13838,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C90">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="D90">
         <v>0.27725856697819312</v>
@@ -13858,7 +13858,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C91">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="D91">
         <v>0.28037383177570091</v>
@@ -13878,7 +13878,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C92">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="D92">
         <v>0.2834890965732087</v>
@@ -13898,7 +13898,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C93">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="D93">
         <v>0.28660436137071649</v>
@@ -13918,7 +13918,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C94">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="D94">
         <v>0.28971962616822428</v>
@@ -13938,7 +13938,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C95">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="D95">
         <v>0.29283489096573206</v>
@@ -13958,7 +13958,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C96">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="D96">
         <v>0.29595015576323985</v>
@@ -13978,7 +13978,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C97">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="D97">
         <v>0.29906542056074764</v>
@@ -13998,7 +13998,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C98">
-        <v>97</v>
+        <v>156</v>
       </c>
       <c r="D98">
         <v>0.30218068535825543</v>
@@ -14018,7 +14018,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C99">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="D99">
         <v>0.30529595015576322</v>
@@ -14038,7 +14038,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C100">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="D100">
         <v>0.30841121495327101</v>
@@ -14058,7 +14058,7 @@
         <v>4.2766661190160553</v>
       </c>
       <c r="C101">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="D101">
         <v>0.3115264797507788</v>
@@ -14078,7 +14078,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C102">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="D102">
         <v>0.31464174454828658</v>
@@ -14098,7 +14098,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C103">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="D103">
         <v>0.31775700934579437</v>
@@ -14118,7 +14118,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C104">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="D104">
         <v>0.32087227414330216</v>
@@ -14138,7 +14138,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C105">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D105">
         <v>0.32398753894080995</v>
@@ -14158,7 +14158,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C106">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="D106">
         <v>0.32710280373831774</v>
@@ -14178,7 +14178,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C107">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="D107">
         <v>0.33021806853582553</v>
@@ -14198,7 +14198,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C108">
-        <v>107</v>
+        <v>166</v>
       </c>
       <c r="D108">
         <v>0.33333333333333331</v>
@@ -14218,7 +14218,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C109">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="D109">
         <v>0.3364485981308411</v>
@@ -14238,7 +14238,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C110">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="D110">
         <v>0.33956386292834889</v>
@@ -14258,7 +14258,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C111">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="D111">
         <v>0.34267912772585668</v>
@@ -14278,7 +14278,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C112">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="D112">
         <v>0.34579439252336447</v>
@@ -14298,7 +14298,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C113">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="D113">
         <v>0.34890965732087226</v>
@@ -14318,7 +14318,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C114">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="D114">
         <v>0.35202492211838005</v>
@@ -14338,7 +14338,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C115">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="D115">
         <v>0.35514018691588783</v>
@@ -14358,7 +14358,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C116">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="D116">
         <v>0.35825545171339562</v>
@@ -14378,7 +14378,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C117">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="D117">
         <v>0.36137071651090341</v>
@@ -14398,7 +14398,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C118">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="D118">
         <v>0.3644859813084112</v>
@@ -14418,7 +14418,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C119">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="D119">
         <v>0.36760124610591899</v>
@@ -14438,7 +14438,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C120">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="D120">
         <v>0.37071651090342678</v>
@@ -14458,7 +14458,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C121">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="D121">
         <v>0.37383177570093457</v>
@@ -14478,7 +14478,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C122">
-        <v>121</v>
+        <v>180</v>
       </c>
       <c r="D122">
         <v>0.37694704049844235</v>
@@ -14498,7 +14498,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C123">
-        <v>122</v>
+        <v>181</v>
       </c>
       <c r="D123">
         <v>0.38006230529595014</v>
@@ -14518,7 +14518,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C124">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="D124">
         <v>0.38317757009345793</v>
@@ -14538,7 +14538,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C125">
-        <v>124</v>
+        <v>183</v>
       </c>
       <c r="D125">
         <v>0.38629283489096572</v>
@@ -14558,7 +14558,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C126">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="D126">
         <v>0.38940809968847351</v>
@@ -14578,7 +14578,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C127">
-        <v>126</v>
+        <v>185</v>
       </c>
       <c r="D127">
         <v>0.3925233644859813</v>
@@ -14598,7 +14598,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C128">
-        <v>127</v>
+        <v>186</v>
       </c>
       <c r="D128">
         <v>0.39563862928348908</v>
@@ -14618,7 +14618,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C129">
-        <v>128</v>
+        <v>187</v>
       </c>
       <c r="D129">
         <v>0.39875389408099687</v>
@@ -14638,7 +14638,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C130">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="D130">
         <v>0.40186915887850466</v>
@@ -14658,7 +14658,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C131">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="D131">
         <v>0.40498442367601245</v>
@@ -14678,7 +14678,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C132">
-        <v>131</v>
+        <v>190</v>
       </c>
       <c r="D132">
         <v>0.40809968847352024</v>
@@ -14698,7 +14698,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C133">
-        <v>132</v>
+        <v>191</v>
       </c>
       <c r="D133">
         <v>0.41121495327102803</v>
@@ -14718,7 +14718,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C134">
-        <v>133</v>
+        <v>192</v>
       </c>
       <c r="D134">
         <v>0.41433021806853582</v>
@@ -14738,7 +14738,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C135">
-        <v>134</v>
+        <v>193</v>
       </c>
       <c r="D135">
         <v>0.4174454828660436</v>
@@ -14758,7 +14758,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C136">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="D136">
         <v>0.42056074766355139</v>
@@ -14778,7 +14778,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C137">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D137">
         <v>0.42367601246105918</v>
@@ -14798,7 +14798,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C138">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="D138">
         <v>0.42679127725856697</v>
@@ -14818,7 +14818,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C139">
-        <v>138</v>
+        <v>197</v>
       </c>
       <c r="D139">
         <v>0.42990654205607476</v>
@@ -14838,7 +14838,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C140">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="D140">
         <v>0.43302180685358255</v>
@@ -14858,7 +14858,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C141">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="D141">
         <v>0.43613707165109034</v>
@@ -14878,7 +14878,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C142">
-        <v>141</v>
+        <v>200</v>
       </c>
       <c r="D142">
         <v>0.43925233644859812</v>
@@ -14898,7 +14898,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C143">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="D143">
         <v>0.44236760124610591</v>
@@ -14918,7 +14918,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C144">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="D144">
         <v>0.4454828660436137</v>
@@ -14938,7 +14938,7 @@
         <v>4.3040650932041693</v>
       </c>
       <c r="C145">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="D145">
         <v>0.44859813084112149</v>
@@ -14958,7 +14958,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C146">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="D146">
         <v>0.45171339563862928</v>
@@ -14978,7 +14978,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C147">
-        <v>146</v>
+        <v>205</v>
       </c>
       <c r="D147">
         <v>0.45482866043613707</v>
@@ -14998,7 +14998,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C148">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="D148">
         <v>0.45794392523364486</v>
@@ -15018,7 +15018,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C149">
-        <v>148</v>
+        <v>207</v>
       </c>
       <c r="D149">
         <v>0.46105919003115264</v>
@@ -15038,7 +15038,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C150">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="D150">
         <v>0.46417445482866043</v>
@@ -15058,7 +15058,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C151">
-        <v>150</v>
+        <v>209</v>
       </c>
       <c r="D151">
         <v>0.46728971962616822</v>
@@ -15078,7 +15078,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C152">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="D152">
         <v>0.47040498442367601</v>
@@ -15098,7 +15098,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C153">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="D153">
         <v>0.4735202492211838</v>
@@ -15118,7 +15118,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C154">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="D154">
         <v>0.47663551401869159</v>
@@ -15138,7 +15138,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C155">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="D155">
         <v>0.47975077881619937</v>
@@ -15158,7 +15158,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C156">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="D156">
         <v>0.48286604361370716</v>
@@ -15178,7 +15178,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C157">
-        <v>156</v>
+        <v>215</v>
       </c>
       <c r="D157">
         <v>0.48598130841121495</v>
@@ -15198,7 +15198,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C158">
-        <v>157</v>
+        <v>216</v>
       </c>
       <c r="D158">
         <v>0.48909657320872274</v>
@@ -15218,7 +15218,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C159">
-        <v>158</v>
+        <v>217</v>
       </c>
       <c r="D159">
         <v>0.49221183800623053</v>
@@ -15238,7 +15238,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C160">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="D160">
         <v>0.49532710280373832</v>
@@ -15258,7 +15258,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C161">
-        <v>160</v>
+        <v>219</v>
       </c>
       <c r="D161">
         <v>0.49844236760124611</v>
@@ -15278,7 +15278,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C162">
-        <v>161</v>
+        <v>220</v>
       </c>
       <c r="D162">
         <v>0.50155763239875384</v>
@@ -15298,7 +15298,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C163">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="D163">
         <v>0.50467289719626163</v>
@@ -15318,7 +15318,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C164">
-        <v>163</v>
+        <v>222</v>
       </c>
       <c r="D164">
         <v>0.50778816199376942</v>
@@ -15338,7 +15338,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C165">
-        <v>164</v>
+        <v>223</v>
       </c>
       <c r="D165">
         <v>0.5109034267912772</v>
@@ -15358,7 +15358,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C166">
-        <v>165</v>
+        <v>224</v>
       </c>
       <c r="D166">
         <v>0.51401869158878499</v>
@@ -15378,7 +15378,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C167">
-        <v>166</v>
+        <v>225</v>
       </c>
       <c r="D167">
         <v>0.51713395638629278</v>
@@ -15398,7 +15398,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C168">
-        <v>167</v>
+        <v>226</v>
       </c>
       <c r="D168">
         <v>0.52024922118380057</v>
@@ -15418,7 +15418,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C169">
-        <v>168</v>
+        <v>227</v>
       </c>
       <c r="D169">
         <v>0.52336448598130836</v>
@@ -15438,7 +15438,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C170">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="D170">
         <v>0.52647975077881615</v>
@@ -15458,7 +15458,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C171">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="D171">
         <v>0.52959501557632394</v>
@@ -15478,7 +15478,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C172">
-        <v>171</v>
+        <v>230</v>
       </c>
       <c r="D172">
         <v>0.53271028037383172</v>
@@ -15498,7 +15498,7 @@
         <v>4.3307333402863311</v>
       </c>
       <c r="C173">
-        <v>172</v>
+        <v>231</v>
       </c>
       <c r="D173">
         <v>0.53582554517133951</v>
@@ -15518,7 +15518,7 @@
         <v>4.3438054218536841</v>
       </c>
       <c r="C174">
-        <v>173</v>
+        <v>232</v>
       </c>
       <c r="D174">
         <v>0.5389408099688473</v>
@@ -15538,7 +15538,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C175">
-        <v>174</v>
+        <v>233</v>
       </c>
       <c r="D175">
         <v>0.54205607476635509</v>
@@ -15558,7 +15558,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C176">
-        <v>175</v>
+        <v>234</v>
       </c>
       <c r="D176">
         <v>0.54517133956386288</v>
@@ -15578,7 +15578,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C177">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="D177">
         <v>0.54828660436137067</v>
@@ -15598,7 +15598,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C178">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="D178">
         <v>0.55140186915887845</v>
@@ -15618,7 +15618,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C179">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="D179">
         <v>0.55451713395638624</v>
@@ -15638,7 +15638,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C180">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="D180">
         <v>0.55763239875389403</v>
@@ -15658,7 +15658,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C181">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="D181">
         <v>0.56074766355140182</v>
@@ -15678,7 +15678,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C182">
-        <v>181</v>
+        <v>240</v>
       </c>
       <c r="D182">
         <v>0.56386292834890961</v>
@@ -15698,7 +15698,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C183">
-        <v>182</v>
+        <v>241</v>
       </c>
       <c r="D183">
         <v>0.5669781931464174</v>
@@ -15718,7 +15718,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C184">
-        <v>183</v>
+        <v>242</v>
       </c>
       <c r="D184">
         <v>0.57009345794392519</v>
@@ -15738,7 +15738,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C185">
-        <v>184</v>
+        <v>243</v>
       </c>
       <c r="D185">
         <v>0.57320872274143297</v>
@@ -15758,7 +15758,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C186">
-        <v>185</v>
+        <v>244</v>
       </c>
       <c r="D186">
         <v>0.57632398753894076</v>
@@ -15778,7 +15778,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C187">
-        <v>186</v>
+        <v>245</v>
       </c>
       <c r="D187">
         <v>0.57943925233644855</v>
@@ -15798,7 +15798,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C188">
-        <v>187</v>
+        <v>246</v>
       </c>
       <c r="D188">
         <v>0.58255451713395634</v>
@@ -15818,7 +15818,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C189">
-        <v>188</v>
+        <v>247</v>
       </c>
       <c r="D189">
         <v>0.58566978193146413</v>
@@ -15838,7 +15838,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C190">
-        <v>189</v>
+        <v>248</v>
       </c>
       <c r="D190">
         <v>0.58878504672897192</v>
@@ -15858,7 +15858,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C191">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="D191">
         <v>0.59190031152647971</v>
@@ -15878,7 +15878,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C192">
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="D192">
         <v>0.59501557632398749</v>
@@ -15898,7 +15898,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C193">
-        <v>192</v>
+        <v>251</v>
       </c>
       <c r="D193">
         <v>0.59813084112149528</v>
@@ -15918,7 +15918,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C194">
-        <v>193</v>
+        <v>252</v>
       </c>
       <c r="D194">
         <v>0.60124610591900307</v>
@@ -15938,7 +15938,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C195">
-        <v>194</v>
+        <v>253</v>
       </c>
       <c r="D195">
         <v>0.60436137071651086</v>
@@ -15958,7 +15958,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C196">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="D196">
         <v>0.60747663551401865</v>
@@ -15978,7 +15978,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C197">
-        <v>196</v>
+        <v>255</v>
       </c>
       <c r="D197">
         <v>0.61059190031152644</v>
@@ -15998,7 +15998,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C198">
-        <v>197</v>
+        <v>256</v>
       </c>
       <c r="D198">
         <v>0.61370716510903423</v>
@@ -16018,7 +16018,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C199">
-        <v>198</v>
+        <v>257</v>
       </c>
       <c r="D199">
         <v>0.61682242990654201</v>
@@ -16038,7 +16038,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C200">
-        <v>199</v>
+        <v>258</v>
       </c>
       <c r="D200">
         <v>0.6199376947040498</v>
@@ -16058,7 +16058,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C201">
-        <v>200</v>
+        <v>259</v>
       </c>
       <c r="D201">
         <v>0.62305295950155759</v>
@@ -16078,7 +16078,7 @@
         <v>4.3567088266895917</v>
       </c>
       <c r="C202">
-        <v>201</v>
+        <v>260</v>
       </c>
       <c r="D202">
         <v>0.62616822429906538</v>
@@ -16098,7 +16098,7 @@
         <v>4.3694478524670215</v>
       </c>
       <c r="C203">
-        <v>202</v>
+        <v>261</v>
       </c>
       <c r="D203">
         <v>0.62928348909657317</v>
@@ -16118,7 +16118,7 @@
         <v>4.3694478524670215</v>
       </c>
       <c r="C204">
-        <v>203</v>
+        <v>262</v>
       </c>
       <c r="D204">
         <v>0.63239875389408096</v>
@@ -16138,7 +16138,7 @@
         <v>4.3694478524670215</v>
       </c>
       <c r="C205">
-        <v>204</v>
+        <v>263</v>
       </c>
       <c r="D205">
         <v>0.63551401869158874</v>
@@ -16158,7 +16158,7 @@
         <v>4.3694478524670215</v>
       </c>
       <c r="C206">
-        <v>205</v>
+        <v>264</v>
       </c>
       <c r="D206">
         <v>0.63862928348909653</v>
@@ -16178,7 +16178,7 @@
         <v>4.3694478524670215</v>
       </c>
       <c r="C207">
-        <v>206</v>
+        <v>265</v>
       </c>
       <c r="D207">
         <v>0.64174454828660432</v>
@@ -16198,7 +16198,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C208">
-        <v>207</v>
+        <v>266</v>
       </c>
       <c r="D208">
         <v>0.64485981308411211</v>
@@ -16218,7 +16218,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C209">
-        <v>208</v>
+        <v>267</v>
       </c>
       <c r="D209">
         <v>0.6479750778816199</v>
@@ -16238,7 +16238,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C210">
-        <v>209</v>
+        <v>268</v>
       </c>
       <c r="D210">
         <v>0.65109034267912769</v>
@@ -16258,7 +16258,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C211">
-        <v>210</v>
+        <v>269</v>
       </c>
       <c r="D211">
         <v>0.65420560747663548</v>
@@ -16278,7 +16278,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C212">
-        <v>211</v>
+        <v>270</v>
       </c>
       <c r="D212">
         <v>0.65732087227414326</v>
@@ -16298,7 +16298,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C213">
-        <v>212</v>
+        <v>271</v>
       </c>
       <c r="D213">
         <v>0.66043613707165105</v>
@@ -16318,7 +16318,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C214">
-        <v>213</v>
+        <v>272</v>
       </c>
       <c r="D214">
         <v>0.66355140186915884</v>
@@ -16338,7 +16338,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C215">
-        <v>214</v>
+        <v>273</v>
       </c>
       <c r="D215">
         <v>0.66666666666666663</v>
@@ -16358,7 +16358,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C216">
-        <v>215</v>
+        <v>274</v>
       </c>
       <c r="D216">
         <v>0.66978193146417442</v>
@@ -16378,7 +16378,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C217">
-        <v>216</v>
+        <v>275</v>
       </c>
       <c r="D217">
         <v>0.67289719626168221</v>
@@ -16398,7 +16398,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C218">
-        <v>217</v>
+        <v>276</v>
       </c>
       <c r="D218">
         <v>0.67601246105919</v>
@@ -16418,7 +16418,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C219">
-        <v>218</v>
+        <v>277</v>
       </c>
       <c r="D219">
         <v>0.67912772585669778</v>
@@ -16438,7 +16438,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C220">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="D220">
         <v>0.68224299065420557</v>
@@ -16458,7 +16458,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C221">
-        <v>220</v>
+        <v>279</v>
       </c>
       <c r="D221">
         <v>0.68535825545171336</v>
@@ -16478,7 +16478,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C222">
-        <v>221</v>
+        <v>280</v>
       </c>
       <c r="D222">
         <v>0.68847352024922115</v>
@@ -16498,7 +16498,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C223">
-        <v>222</v>
+        <v>281</v>
       </c>
       <c r="D223">
         <v>0.69158878504672894</v>
@@ -16518,7 +16518,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C224">
-        <v>223</v>
+        <v>282</v>
       </c>
       <c r="D224">
         <v>0.69470404984423673</v>
@@ -16538,7 +16538,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C225">
-        <v>224</v>
+        <v>283</v>
       </c>
       <c r="D225">
         <v>0.69781931464174451</v>
@@ -16558,7 +16558,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C226">
-        <v>225</v>
+        <v>284</v>
       </c>
       <c r="D226">
         <v>0.7009345794392523</v>
@@ -16578,7 +16578,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C227">
-        <v>226</v>
+        <v>285</v>
       </c>
       <c r="D227">
         <v>0.70404984423676009</v>
@@ -16598,7 +16598,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C228">
-        <v>227</v>
+        <v>286</v>
       </c>
       <c r="D228">
         <v>0.70716510903426788</v>
@@ -16618,7 +16618,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C229">
-        <v>228</v>
+        <v>287</v>
       </c>
       <c r="D229">
         <v>0.71028037383177567</v>
@@ -16638,7 +16638,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C230">
-        <v>229</v>
+        <v>288</v>
       </c>
       <c r="D230">
         <v>0.71339563862928346</v>
@@ -16658,7 +16658,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C231">
-        <v>230</v>
+        <v>289</v>
       </c>
       <c r="D231">
         <v>0.71651090342679125</v>
@@ -16678,7 +16678,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C232">
-        <v>231</v>
+        <v>290</v>
       </c>
       <c r="D232">
         <v>0.71962616822429903</v>
@@ -16698,7 +16698,7 @@
         <v>4.3820266346738812</v>
       </c>
       <c r="C233">
-        <v>232</v>
+        <v>291</v>
       </c>
       <c r="D233">
         <v>0.72274143302180682</v>
@@ -16718,7 +16718,7 @@
         <v>4.3944491546724391</v>
       </c>
       <c r="C234">
-        <v>233</v>
+        <v>292</v>
       </c>
       <c r="D234">
         <v>0.72585669781931461</v>
@@ -16738,7 +16738,7 @@
         <v>4.3944491546724391</v>
       </c>
       <c r="C235">
-        <v>234</v>
+        <v>293</v>
       </c>
       <c r="D235">
         <v>0.7289719626168224</v>
@@ -16758,7 +16758,7 @@
         <v>4.3944491546724391</v>
       </c>
       <c r="C236">
-        <v>235</v>
+        <v>294</v>
       </c>
       <c r="D236">
         <v>0.73208722741433019</v>
@@ -16778,7 +16778,7 @@
         <v>4.3944491546724391</v>
       </c>
       <c r="C237">
-        <v>236</v>
+        <v>295</v>
       </c>
       <c r="D237">
         <v>0.73520249221183798</v>
@@ -16798,7 +16798,7 @@
         <v>4.3944491546724391</v>
       </c>
       <c r="C238">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="D238">
         <v>0.73831775700934577</v>
@@ -16818,7 +16818,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C239">
-        <v>238</v>
+        <v>297</v>
       </c>
       <c r="D239">
         <v>0.74143302180685355</v>
@@ -16838,7 +16838,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C240">
-        <v>239</v>
+        <v>298</v>
       </c>
       <c r="D240">
         <v>0.74454828660436134</v>
@@ -16858,7 +16858,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C241">
-        <v>240</v>
+        <v>299</v>
       </c>
       <c r="D241">
         <v>0.74766355140186913</v>
@@ -16878,7 +16878,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C242">
-        <v>241</v>
+        <v>300</v>
       </c>
       <c r="D242">
         <v>0.75077881619937692</v>
@@ -16898,7 +16898,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C243">
-        <v>242</v>
+        <v>301</v>
       </c>
       <c r="D243">
         <v>0.75389408099688471</v>
@@ -16918,7 +16918,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C244">
-        <v>243</v>
+        <v>302</v>
       </c>
       <c r="D244">
         <v>0.7570093457943925</v>
@@ -16938,7 +16938,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C245">
-        <v>244</v>
+        <v>303</v>
       </c>
       <c r="D245">
         <v>0.76012461059190028</v>
@@ -16958,7 +16958,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C246">
-        <v>245</v>
+        <v>304</v>
       </c>
       <c r="D246">
         <v>0.76323987538940807</v>
@@ -16978,7 +16978,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C247">
-        <v>246</v>
+        <v>305</v>
       </c>
       <c r="D247">
         <v>0.76635514018691586</v>
@@ -16998,7 +16998,7 @@
         <v>4.4067192472642533</v>
       </c>
       <c r="C248">
-        <v>247</v>
+        <v>306</v>
       </c>
       <c r="D248">
         <v>0.76947040498442365</v>
@@ -17018,7 +17018,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C249">
-        <v>248</v>
+        <v>307</v>
       </c>
       <c r="D249">
         <v>0.77258566978193144</v>
@@ -17038,7 +17038,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C250">
-        <v>249</v>
+        <v>308</v>
       </c>
       <c r="D250">
         <v>0.77570093457943923</v>
@@ -17058,7 +17058,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C251">
-        <v>250</v>
+        <v>309</v>
       </c>
       <c r="D251">
         <v>0.77881619937694702</v>
@@ -17078,7 +17078,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C252">
-        <v>251</v>
+        <v>310</v>
       </c>
       <c r="D252">
         <v>0.7819314641744548</v>
@@ -17098,7 +17098,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C253">
-        <v>252</v>
+        <v>311</v>
       </c>
       <c r="D253">
         <v>0.78504672897196259</v>
@@ -17118,7 +17118,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C254">
-        <v>253</v>
+        <v>312</v>
       </c>
       <c r="D254">
         <v>0.78816199376947038</v>
@@ -17138,7 +17138,7 @@
         <v>4.4188406077965983</v>
       </c>
       <c r="C255">
-        <v>254</v>
+        <v>313</v>
       </c>
       <c r="D255">
         <v>0.79127725856697817</v>
@@ -17158,7 +17158,7 @@
         <v>4.4308167988433134</v>
       </c>
       <c r="C256">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="D256">
         <v>0.79439252336448596</v>
@@ -17178,7 +17178,7 @@
         <v>4.4308167988433134</v>
       </c>
       <c r="C257">
-        <v>256</v>
+        <v>315</v>
       </c>
       <c r="D257">
         <v>0.79750778816199375</v>
@@ -17198,7 +17198,7 @@
         <v>4.4426512564903167</v>
       </c>
       <c r="C258">
-        <v>257</v>
+        <v>316</v>
       </c>
       <c r="D258">
         <v>0.80062305295950154</v>
@@ -17218,7 +17218,7 @@
         <v>4.4426512564903167</v>
       </c>
       <c r="C259">
-        <v>258</v>
+        <v>317</v>
       </c>
       <c r="D259">
         <v>0.80373831775700932</v>
@@ -17238,7 +17238,7 @@
         <v>4.4426512564903167</v>
       </c>
       <c r="C260">
-        <v>259</v>
+        <v>318</v>
       </c>
       <c r="D260">
         <v>0.80685358255451711</v>
@@ -17258,7 +17258,7 @@
         <v>4.4426512564903167</v>
       </c>
       <c r="C261">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="D261">
         <v>0.8099688473520249</v>
@@ -17278,7 +17278,7 @@
         <v>4.4426512564903167</v>
       </c>
       <c r="C262">
-        <v>261</v>
+        <v>320</v>
       </c>
       <c r="D262">
         <v>0.81308411214953269</v>
@@ -17298,7 +17298,7 @@
         <v>4.4426512564903167</v>
       </c>
       <c r="C263">
-        <v>262</v>
+        <v>321</v>
       </c>
       <c r="D263">
         <v>0.81619937694704048</v>
@@ -17318,7 +17318,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C264">
-        <v>263</v>
+        <v>322</v>
       </c>
       <c r="D264">
         <v>0.81931464174454827</v>
@@ -17338,7 +17338,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C265">
-        <v>264</v>
+        <v>323</v>
       </c>
       <c r="D265">
         <v>0.82242990654205606</v>
@@ -17358,7 +17358,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C266">
-        <v>265</v>
+        <v>324</v>
       </c>
       <c r="D266">
         <v>0.82554517133956384</v>
@@ -17378,7 +17378,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C267">
-        <v>266</v>
+        <v>325</v>
       </c>
       <c r="D267">
         <v>0.82866043613707163</v>
@@ -17398,7 +17398,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C268">
-        <v>267</v>
+        <v>326</v>
       </c>
       <c r="D268">
         <v>0.83177570093457942</v>
@@ -17418,7 +17418,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C269">
-        <v>268</v>
+        <v>327</v>
       </c>
       <c r="D269">
         <v>0.83489096573208721</v>
@@ -17438,7 +17438,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="C270">
-        <v>269</v>
+        <v>328</v>
       </c>
       <c r="D270">
         <v>0.838006230529595</v>
@@ -17458,7 +17458,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C271">
-        <v>270</v>
+        <v>329</v>
       </c>
       <c r="D271">
         <v>0.84112149532710279</v>
@@ -17478,7 +17478,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C272">
-        <v>271</v>
+        <v>330</v>
       </c>
       <c r="D272">
         <v>0.84423676012461057</v>
@@ -17498,7 +17498,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C273">
-        <v>272</v>
+        <v>331</v>
       </c>
       <c r="D273">
         <v>0.84735202492211836</v>
@@ -17518,7 +17518,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C274">
-        <v>273</v>
+        <v>332</v>
       </c>
       <c r="D274">
         <v>0.85046728971962615</v>
@@ -17538,7 +17538,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C275">
-        <v>274</v>
+        <v>333</v>
       </c>
       <c r="D275">
         <v>0.85358255451713394</v>
@@ -17558,7 +17558,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C276">
-        <v>275</v>
+        <v>334</v>
       </c>
       <c r="D276">
         <v>0.85669781931464173</v>
@@ -17578,7 +17578,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C277">
-        <v>276</v>
+        <v>335</v>
       </c>
       <c r="D277">
         <v>0.85981308411214952</v>
@@ -17598,7 +17598,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C278">
-        <v>277</v>
+        <v>336</v>
       </c>
       <c r="D278">
         <v>0.86292834890965731</v>
@@ -17618,7 +17618,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C279">
-        <v>278</v>
+        <v>337</v>
       </c>
       <c r="D279">
         <v>0.86604361370716509</v>
@@ -17638,7 +17638,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C280">
-        <v>279</v>
+        <v>338</v>
       </c>
       <c r="D280">
         <v>0.86915887850467288</v>
@@ -17658,7 +17658,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C281">
-        <v>280</v>
+        <v>339</v>
       </c>
       <c r="D281">
         <v>0.87227414330218067</v>
@@ -17678,7 +17678,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C282">
-        <v>281</v>
+        <v>340</v>
       </c>
       <c r="D282">
         <v>0.87538940809968846</v>
@@ -17698,7 +17698,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C283">
-        <v>282</v>
+        <v>341</v>
       </c>
       <c r="D283">
         <v>0.87850467289719625</v>
@@ -17718,7 +17718,7 @@
         <v>4.4886363697321396</v>
       </c>
       <c r="C284">
-        <v>283</v>
+        <v>342</v>
       </c>
       <c r="D284">
         <v>0.88161993769470404</v>
@@ -17738,7 +17738,7 @@
         <v>4.499809670330265</v>
       </c>
       <c r="C285">
-        <v>284</v>
+        <v>343</v>
       </c>
       <c r="D285">
         <v>0.88473520249221183</v>
@@ -17758,7 +17758,7 @@
         <v>4.499809670330265</v>
       </c>
       <c r="C286">
-        <v>285</v>
+        <v>344</v>
       </c>
       <c r="D286">
         <v>0.88785046728971961</v>
@@ -17778,7 +17778,7 @@
         <v>4.5108595065168497</v>
       </c>
       <c r="C287">
-        <v>286</v>
+        <v>345</v>
       </c>
       <c r="D287">
         <v>0.8909657320872274</v>
@@ -17798,7 +17798,7 @@
         <v>4.5108595065168497</v>
       </c>
       <c r="C288">
-        <v>287</v>
+        <v>346</v>
       </c>
       <c r="D288">
         <v>0.89408099688473519</v>
@@ -17818,7 +17818,7 @@
         <v>4.5108595065168497</v>
       </c>
       <c r="C289">
-        <v>288</v>
+        <v>347</v>
       </c>
       <c r="D289">
         <v>0.89719626168224298</v>
@@ -17838,7 +17838,7 @@
         <v>4.5108595065168497</v>
       </c>
       <c r="C290">
-        <v>289</v>
+        <v>348</v>
       </c>
       <c r="D290">
         <v>0.90031152647975077</v>
@@ -17858,7 +17858,7 @@
         <v>4.5325994931532563</v>
       </c>
       <c r="C291">
-        <v>290</v>
+        <v>349</v>
       </c>
       <c r="D291">
         <v>0.90342679127725856</v>
@@ -17878,7 +17878,7 @@
         <v>4.5325994931532563</v>
       </c>
       <c r="C292">
-        <v>291</v>
+        <v>350</v>
       </c>
       <c r="D292">
         <v>0.90654205607476634</v>
@@ -17898,7 +17898,7 @@
         <v>4.5325994931532563</v>
       </c>
       <c r="C293">
-        <v>292</v>
+        <v>351</v>
       </c>
       <c r="D293">
         <v>0.90965732087227413</v>
@@ -17918,7 +17918,7 @@
         <v>4.5325994931532563</v>
       </c>
       <c r="C294">
-        <v>293</v>
+        <v>352</v>
       </c>
       <c r="D294">
         <v>0.91277258566978192</v>
@@ -17938,7 +17938,7 @@
         <v>4.5538768916005408</v>
       </c>
       <c r="C295">
-        <v>294</v>
+        <v>353</v>
       </c>
       <c r="D295">
         <v>0.91588785046728971</v>
@@ -17958,7 +17958,7 @@
         <v>4.5538768916005408</v>
       </c>
       <c r="C296">
-        <v>295</v>
+        <v>354</v>
       </c>
       <c r="D296">
         <v>0.9190031152647975</v>
@@ -17978,7 +17978,7 @@
         <v>4.5538768916005408</v>
       </c>
       <c r="C297">
-        <v>296</v>
+        <v>355</v>
       </c>
       <c r="D297">
         <v>0.92211838006230529</v>
@@ -17998,7 +17998,7 @@
         <v>4.5643481914678361</v>
       </c>
       <c r="C298">
-        <v>297</v>
+        <v>356</v>
       </c>
       <c r="D298">
         <v>0.92523364485981308</v>
@@ -18018,7 +18018,7 @@
         <v>4.5643481914678361</v>
       </c>
       <c r="C299">
-        <v>298</v>
+        <v>357</v>
       </c>
       <c r="D299">
         <v>0.92834890965732086</v>
@@ -18038,7 +18038,7 @@
         <v>4.5643481914678361</v>
       </c>
       <c r="C300">
-        <v>299</v>
+        <v>358</v>
       </c>
       <c r="D300">
         <v>0.93146417445482865</v>
@@ -18058,7 +18058,7 @@
         <v>4.5643481914678361</v>
       </c>
       <c r="C301">
-        <v>300</v>
+        <v>359</v>
       </c>
       <c r="D301">
         <v>0.93457943925233644</v>
@@ -18078,7 +18078,7 @@
         <v>4.5643481914678361</v>
       </c>
       <c r="C302">
-        <v>301</v>
+        <v>360</v>
       </c>
       <c r="D302">
         <v>0.93769470404984423</v>
@@ -18098,7 +18098,7 @@
         <v>4.5849674786705723</v>
       </c>
       <c r="C303">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="D303">
         <v>0.94080996884735202</v>
@@ -18118,7 +18118,7 @@
         <v>4.5849674786705723</v>
       </c>
       <c r="C304">
-        <v>303</v>
+        <v>362</v>
       </c>
       <c r="D304">
         <v>0.94392523364485981</v>
@@ -18138,7 +18138,7 @@
         <v>4.5849674786705723</v>
       </c>
       <c r="C305">
-        <v>304</v>
+        <v>363</v>
       </c>
       <c r="D305">
         <v>0.9470404984423676</v>
@@ -18158,7 +18158,7 @@
         <v>4.6051701859880918</v>
       </c>
       <c r="C306">
-        <v>305</v>
+        <v>364</v>
       </c>
       <c r="D306">
         <v>0.95015576323987538</v>
@@ -18178,7 +18178,7 @@
         <v>4.6051701859880918</v>
       </c>
       <c r="C307">
-        <v>306</v>
+        <v>365</v>
       </c>
       <c r="D307">
         <v>0.95327102803738317</v>
@@ -18198,7 +18198,7 @@
         <v>4.6051701859880918</v>
       </c>
       <c r="C308">
-        <v>307</v>
+        <v>366</v>
       </c>
       <c r="D308">
         <v>0.95638629283489096</v>
@@ -18218,7 +18218,7 @@
         <v>4.6051701859880918</v>
       </c>
       <c r="C309">
-        <v>308</v>
+        <v>367</v>
       </c>
       <c r="D309">
         <v>0.95950155763239875</v>
@@ -18238,7 +18238,7 @@
         <v>4.6151205168412597</v>
       </c>
       <c r="C310">
-        <v>309</v>
+        <v>368</v>
       </c>
       <c r="D310">
         <v>0.96261682242990654</v>
@@ -18258,7 +18258,7 @@
         <v>4.6249728132842707</v>
       </c>
       <c r="C311">
-        <v>310</v>
+        <v>369</v>
       </c>
       <c r="D311">
         <v>0.96573208722741433</v>
@@ -18278,7 +18278,7 @@
         <v>4.6249728132842707</v>
       </c>
       <c r="C312">
-        <v>311</v>
+        <v>370</v>
       </c>
       <c r="D312">
         <v>0.96884735202492211</v>
@@ -18298,7 +18298,7 @@
         <v>4.6443908991413725</v>
       </c>
       <c r="C313">
-        <v>312</v>
+        <v>371</v>
       </c>
       <c r="D313">
         <v>0.9719626168224299</v>
@@ -18318,7 +18318,7 @@
         <v>4.6443908991413725</v>
       </c>
       <c r="C314">
-        <v>313</v>
+        <v>372</v>
       </c>
       <c r="D314">
         <v>0.97507788161993769</v>
@@ -18338,7 +18338,7 @@
         <v>4.6443908991413725</v>
       </c>
       <c r="C315">
-        <v>314</v>
+        <v>373</v>
       </c>
       <c r="D315">
         <v>0.97819314641744548</v>
@@ -18358,7 +18358,7 @@
         <v>4.6634390941120669</v>
       </c>
       <c r="C316">
-        <v>315</v>
+        <v>374</v>
       </c>
       <c r="D316">
         <v>0.98130841121495327</v>
@@ -18378,7 +18378,7 @@
         <v>4.6634390941120669</v>
       </c>
       <c r="C317">
-        <v>316</v>
+        <v>375</v>
       </c>
       <c r="D317">
         <v>0.98442367601246106</v>
@@ -18398,7 +18398,7 @@
         <v>4.6728288344619058</v>
       </c>
       <c r="C318">
-        <v>317</v>
+        <v>376</v>
       </c>
       <c r="D318">
         <v>0.98753894080996885</v>
@@ -18418,7 +18418,7 @@
         <v>4.7095302013123339</v>
       </c>
       <c r="C319">
-        <v>318</v>
+        <v>377</v>
       </c>
       <c r="D319">
         <v>0.99065420560747663</v>
@@ -18438,7 +18438,7 @@
         <v>4.7449321283632502</v>
       </c>
       <c r="C320">
-        <v>319</v>
+        <v>378</v>
       </c>
       <c r="D320">
         <v>0.99376947040498442</v>
@@ -18458,7 +18458,7 @@
         <v>4.9052747784384296</v>
       </c>
       <c r="C321">
-        <v>320</v>
+        <v>379</v>
       </c>
       <c r="D321">
         <v>0.99688473520249221</v>
@@ -18468,6 +18468,1186 @@
       </c>
       <c r="F321">
         <v>1.7529218107091813</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>0</v>
+      </c>
+      <c r="B322">
+        <v>0</v>
+      </c>
+      <c r="C322">
+        <v>321</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+      <c r="E322">
+        <v>0</v>
+      </c>
+      <c r="F322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>0</v>
+      </c>
+      <c r="B323">
+        <v>0</v>
+      </c>
+      <c r="C323">
+        <v>322</v>
+      </c>
+      <c r="D323">
+        <v>0</v>
+      </c>
+      <c r="E323">
+        <v>0</v>
+      </c>
+      <c r="F323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>0</v>
+      </c>
+      <c r="B324">
+        <v>0</v>
+      </c>
+      <c r="C324">
+        <v>323</v>
+      </c>
+      <c r="D324">
+        <v>0</v>
+      </c>
+      <c r="E324">
+        <v>0</v>
+      </c>
+      <c r="F324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>0</v>
+      </c>
+      <c r="B325">
+        <v>0</v>
+      </c>
+      <c r="C325">
+        <v>324</v>
+      </c>
+      <c r="D325">
+        <v>0</v>
+      </c>
+      <c r="E325">
+        <v>0</v>
+      </c>
+      <c r="F325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>0</v>
+      </c>
+      <c r="B326">
+        <v>0</v>
+      </c>
+      <c r="C326">
+        <v>325</v>
+      </c>
+      <c r="D326">
+        <v>0</v>
+      </c>
+      <c r="E326">
+        <v>0</v>
+      </c>
+      <c r="F326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>0</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+      <c r="C327">
+        <v>326</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327">
+        <v>0</v>
+      </c>
+      <c r="F327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>0</v>
+      </c>
+      <c r="B328">
+        <v>0</v>
+      </c>
+      <c r="C328">
+        <v>327</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328">
+        <v>0</v>
+      </c>
+      <c r="F328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>0</v>
+      </c>
+      <c r="B329">
+        <v>0</v>
+      </c>
+      <c r="C329">
+        <v>328</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+      <c r="E329">
+        <v>0</v>
+      </c>
+      <c r="F329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>0</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+      <c r="C330">
+        <v>329</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+      <c r="E330">
+        <v>0</v>
+      </c>
+      <c r="F330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>0</v>
+      </c>
+      <c r="B331">
+        <v>0</v>
+      </c>
+      <c r="C331">
+        <v>330</v>
+      </c>
+      <c r="D331">
+        <v>0</v>
+      </c>
+      <c r="E331">
+        <v>0</v>
+      </c>
+      <c r="F331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>0</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+      <c r="C332">
+        <v>331</v>
+      </c>
+      <c r="D332">
+        <v>0</v>
+      </c>
+      <c r="E332">
+        <v>0</v>
+      </c>
+      <c r="F332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>0</v>
+      </c>
+      <c r="B333">
+        <v>0</v>
+      </c>
+      <c r="C333">
+        <v>332</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333">
+        <v>0</v>
+      </c>
+      <c r="F333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>0</v>
+      </c>
+      <c r="B334">
+        <v>0</v>
+      </c>
+      <c r="C334">
+        <v>333</v>
+      </c>
+      <c r="D334">
+        <v>0</v>
+      </c>
+      <c r="E334">
+        <v>0</v>
+      </c>
+      <c r="F334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>0</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+      <c r="C335">
+        <v>334</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+      <c r="E335">
+        <v>0</v>
+      </c>
+      <c r="F335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>0</v>
+      </c>
+      <c r="B336">
+        <v>0</v>
+      </c>
+      <c r="C336">
+        <v>335</v>
+      </c>
+      <c r="D336">
+        <v>0</v>
+      </c>
+      <c r="E336">
+        <v>0</v>
+      </c>
+      <c r="F336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>0</v>
+      </c>
+      <c r="B337">
+        <v>0</v>
+      </c>
+      <c r="C337">
+        <v>336</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+      <c r="E337">
+        <v>0</v>
+      </c>
+      <c r="F337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>0</v>
+      </c>
+      <c r="B338">
+        <v>0</v>
+      </c>
+      <c r="C338">
+        <v>337</v>
+      </c>
+      <c r="D338">
+        <v>0</v>
+      </c>
+      <c r="E338">
+        <v>0</v>
+      </c>
+      <c r="F338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>0</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <v>338</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+      <c r="E339">
+        <v>0</v>
+      </c>
+      <c r="F339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>0</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+      <c r="C340">
+        <v>339</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+      <c r="E340">
+        <v>0</v>
+      </c>
+      <c r="F340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>0</v>
+      </c>
+      <c r="B341">
+        <v>0</v>
+      </c>
+      <c r="C341">
+        <v>340</v>
+      </c>
+      <c r="D341">
+        <v>0</v>
+      </c>
+      <c r="E341">
+        <v>0</v>
+      </c>
+      <c r="F341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>0</v>
+      </c>
+      <c r="B342">
+        <v>0</v>
+      </c>
+      <c r="C342">
+        <v>341</v>
+      </c>
+      <c r="D342">
+        <v>0</v>
+      </c>
+      <c r="E342">
+        <v>0</v>
+      </c>
+      <c r="F342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>0</v>
+      </c>
+      <c r="B343">
+        <v>0</v>
+      </c>
+      <c r="C343">
+        <v>342</v>
+      </c>
+      <c r="D343">
+        <v>0</v>
+      </c>
+      <c r="E343">
+        <v>0</v>
+      </c>
+      <c r="F343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>0</v>
+      </c>
+      <c r="B344">
+        <v>0</v>
+      </c>
+      <c r="C344">
+        <v>343</v>
+      </c>
+      <c r="D344">
+        <v>0</v>
+      </c>
+      <c r="E344">
+        <v>0</v>
+      </c>
+      <c r="F344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>0</v>
+      </c>
+      <c r="B345">
+        <v>0</v>
+      </c>
+      <c r="C345">
+        <v>344</v>
+      </c>
+      <c r="D345">
+        <v>0</v>
+      </c>
+      <c r="E345">
+        <v>0</v>
+      </c>
+      <c r="F345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>0</v>
+      </c>
+      <c r="B346">
+        <v>0</v>
+      </c>
+      <c r="C346">
+        <v>345</v>
+      </c>
+      <c r="D346">
+        <v>0</v>
+      </c>
+      <c r="E346">
+        <v>0</v>
+      </c>
+      <c r="F346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>0</v>
+      </c>
+      <c r="B347">
+        <v>0</v>
+      </c>
+      <c r="C347">
+        <v>346</v>
+      </c>
+      <c r="D347">
+        <v>0</v>
+      </c>
+      <c r="E347">
+        <v>0</v>
+      </c>
+      <c r="F347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>0</v>
+      </c>
+      <c r="B348">
+        <v>0</v>
+      </c>
+      <c r="C348">
+        <v>347</v>
+      </c>
+      <c r="D348">
+        <v>0</v>
+      </c>
+      <c r="E348">
+        <v>0</v>
+      </c>
+      <c r="F348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>0</v>
+      </c>
+      <c r="B349">
+        <v>0</v>
+      </c>
+      <c r="C349">
+        <v>348</v>
+      </c>
+      <c r="D349">
+        <v>0</v>
+      </c>
+      <c r="E349">
+        <v>0</v>
+      </c>
+      <c r="F349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>0</v>
+      </c>
+      <c r="B350">
+        <v>0</v>
+      </c>
+      <c r="C350">
+        <v>349</v>
+      </c>
+      <c r="D350">
+        <v>0</v>
+      </c>
+      <c r="E350">
+        <v>0</v>
+      </c>
+      <c r="F350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>0</v>
+      </c>
+      <c r="B351">
+        <v>0</v>
+      </c>
+      <c r="C351">
+        <v>350</v>
+      </c>
+      <c r="D351">
+        <v>0</v>
+      </c>
+      <c r="E351">
+        <v>0</v>
+      </c>
+      <c r="F351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>0</v>
+      </c>
+      <c r="B352">
+        <v>0</v>
+      </c>
+      <c r="C352">
+        <v>351</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+      <c r="E352">
+        <v>0</v>
+      </c>
+      <c r="F352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>0</v>
+      </c>
+      <c r="B353">
+        <v>0</v>
+      </c>
+      <c r="C353">
+        <v>352</v>
+      </c>
+      <c r="D353">
+        <v>0</v>
+      </c>
+      <c r="E353">
+        <v>0</v>
+      </c>
+      <c r="F353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>0</v>
+      </c>
+      <c r="B354">
+        <v>0</v>
+      </c>
+      <c r="C354">
+        <v>353</v>
+      </c>
+      <c r="D354">
+        <v>0</v>
+      </c>
+      <c r="E354">
+        <v>0</v>
+      </c>
+      <c r="F354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>0</v>
+      </c>
+      <c r="B355">
+        <v>0</v>
+      </c>
+      <c r="C355">
+        <v>354</v>
+      </c>
+      <c r="D355">
+        <v>0</v>
+      </c>
+      <c r="E355">
+        <v>0</v>
+      </c>
+      <c r="F355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>0</v>
+      </c>
+      <c r="B356">
+        <v>0</v>
+      </c>
+      <c r="C356">
+        <v>355</v>
+      </c>
+      <c r="D356">
+        <v>0</v>
+      </c>
+      <c r="E356">
+        <v>0</v>
+      </c>
+      <c r="F356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>0</v>
+      </c>
+      <c r="B357">
+        <v>0</v>
+      </c>
+      <c r="C357">
+        <v>356</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357">
+        <v>0</v>
+      </c>
+      <c r="F357">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>0</v>
+      </c>
+      <c r="B358">
+        <v>0</v>
+      </c>
+      <c r="C358">
+        <v>357</v>
+      </c>
+      <c r="D358">
+        <v>0</v>
+      </c>
+      <c r="E358">
+        <v>0</v>
+      </c>
+      <c r="F358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>0</v>
+      </c>
+      <c r="B359">
+        <v>0</v>
+      </c>
+      <c r="C359">
+        <v>358</v>
+      </c>
+      <c r="D359">
+        <v>0</v>
+      </c>
+      <c r="E359">
+        <v>0</v>
+      </c>
+      <c r="F359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>0</v>
+      </c>
+      <c r="B360">
+        <v>0</v>
+      </c>
+      <c r="C360">
+        <v>359</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+      <c r="E360">
+        <v>0</v>
+      </c>
+      <c r="F360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>0</v>
+      </c>
+      <c r="B361">
+        <v>0</v>
+      </c>
+      <c r="C361">
+        <v>360</v>
+      </c>
+      <c r="D361">
+        <v>0</v>
+      </c>
+      <c r="E361">
+        <v>0</v>
+      </c>
+      <c r="F361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>0</v>
+      </c>
+      <c r="B362">
+        <v>0</v>
+      </c>
+      <c r="C362">
+        <v>361</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362">
+        <v>0</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>0</v>
+      </c>
+      <c r="B363">
+        <v>0</v>
+      </c>
+      <c r="C363">
+        <v>362</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363">
+        <v>0</v>
+      </c>
+      <c r="F363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>0</v>
+      </c>
+      <c r="B364">
+        <v>0</v>
+      </c>
+      <c r="C364">
+        <v>363</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>0</v>
+      </c>
+      <c r="F364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>0</v>
+      </c>
+      <c r="B365">
+        <v>0</v>
+      </c>
+      <c r="C365">
+        <v>364</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>0</v>
+      </c>
+      <c r="F365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>0</v>
+      </c>
+      <c r="B366">
+        <v>0</v>
+      </c>
+      <c r="C366">
+        <v>365</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>0</v>
+      </c>
+      <c r="F366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>0</v>
+      </c>
+      <c r="B367">
+        <v>0</v>
+      </c>
+      <c r="C367">
+        <v>366</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367">
+        <v>0</v>
+      </c>
+      <c r="F367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>0</v>
+      </c>
+      <c r="B368">
+        <v>0</v>
+      </c>
+      <c r="C368">
+        <v>367</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368">
+        <v>0</v>
+      </c>
+      <c r="F368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>0</v>
+      </c>
+      <c r="B369">
+        <v>0</v>
+      </c>
+      <c r="C369">
+        <v>368</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369">
+        <v>0</v>
+      </c>
+      <c r="F369">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>0</v>
+      </c>
+      <c r="B370">
+        <v>0</v>
+      </c>
+      <c r="C370">
+        <v>369</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+      <c r="E370">
+        <v>0</v>
+      </c>
+      <c r="F370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>0</v>
+      </c>
+      <c r="B371">
+        <v>0</v>
+      </c>
+      <c r="C371">
+        <v>370</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371">
+        <v>0</v>
+      </c>
+      <c r="F371">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>0</v>
+      </c>
+      <c r="B372">
+        <v>0</v>
+      </c>
+      <c r="C372">
+        <v>371</v>
+      </c>
+      <c r="D372">
+        <v>0</v>
+      </c>
+      <c r="E372">
+        <v>0</v>
+      </c>
+      <c r="F372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>0</v>
+      </c>
+      <c r="B373">
+        <v>0</v>
+      </c>
+      <c r="C373">
+        <v>372</v>
+      </c>
+      <c r="D373">
+        <v>0</v>
+      </c>
+      <c r="E373">
+        <v>0</v>
+      </c>
+      <c r="F373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>0</v>
+      </c>
+      <c r="B374">
+        <v>0</v>
+      </c>
+      <c r="C374">
+        <v>373</v>
+      </c>
+      <c r="D374">
+        <v>0</v>
+      </c>
+      <c r="E374">
+        <v>0</v>
+      </c>
+      <c r="F374">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>0</v>
+      </c>
+      <c r="B375">
+        <v>0</v>
+      </c>
+      <c r="C375">
+        <v>374</v>
+      </c>
+      <c r="D375">
+        <v>0</v>
+      </c>
+      <c r="E375">
+        <v>0</v>
+      </c>
+      <c r="F375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>0</v>
+      </c>
+      <c r="B376">
+        <v>0</v>
+      </c>
+      <c r="C376">
+        <v>375</v>
+      </c>
+      <c r="D376">
+        <v>0</v>
+      </c>
+      <c r="E376">
+        <v>0</v>
+      </c>
+      <c r="F376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>0</v>
+      </c>
+      <c r="B377">
+        <v>0</v>
+      </c>
+      <c r="C377">
+        <v>376</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>0</v>
+      </c>
+      <c r="F377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>0</v>
+      </c>
+      <c r="B378">
+        <v>0</v>
+      </c>
+      <c r="C378">
+        <v>377</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378">
+        <v>0</v>
+      </c>
+      <c r="F378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>0</v>
+      </c>
+      <c r="B379">
+        <v>0</v>
+      </c>
+      <c r="C379">
+        <v>378</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379">
+        <v>0</v>
+      </c>
+      <c r="F379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>0</v>
+      </c>
+      <c r="B380">
+        <v>0</v>
+      </c>
+      <c r="C380">
+        <v>379</v>
+      </c>
+      <c r="D380">
+        <v>0</v>
+      </c>
+      <c r="E380">
+        <v>0</v>
+      </c>
+      <c r="F380">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>